<commit_message>
Updated from meeting 4/27
</commit_message>
<xml_diff>
--- a/HornetNewDataWithPositiveCases.xlsx
+++ b/HornetNewDataWithPositiveCases.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hreed\Documents\UCF\Projects\Hornet-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEC2AA7-B52F-4A0A-B2AB-DADA795AEF93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E12DEF-34AB-4700-9605-01AA01842E54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{88050B78-2E05-C04B-8432-556A30D89647}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6572510-426F-2E42-B2E9-009B1A7EC2C3}">
   <dimension ref="A1:E799"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A788" workbookViewId="0">
-      <selection activeCell="E723" sqref="E723"/>
+    <sheetView tabSelected="1" topLeftCell="A773" workbookViewId="0">
+      <selection activeCell="F723" sqref="F723"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -869,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -2076,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="E97" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
@@ -2637,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="E130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -3385,7 +3385,7 @@
         <v>1</v>
       </c>
       <c r="E174" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
@@ -8043,7 +8043,7 @@
         <v>1</v>
       </c>
       <c r="E448" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.35">
@@ -11800,7 +11800,7 @@
         <v>1</v>
       </c>
       <c r="E669" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="670" spans="1:5" x14ac:dyDescent="0.35">
@@ -12378,7 +12378,7 @@
         <v>1</v>
       </c>
       <c r="E703" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="704" spans="1:5" x14ac:dyDescent="0.35">
@@ -12497,7 +12497,7 @@
         <v>1</v>
       </c>
       <c r="E710" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="711" spans="1:5" x14ac:dyDescent="0.35">
@@ -12633,7 +12633,7 @@
         <v>1</v>
       </c>
       <c r="E718" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="719" spans="1:5" x14ac:dyDescent="0.35">
@@ -12718,7 +12718,7 @@
         <v>1</v>
       </c>
       <c r="E723" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="724" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>